<commit_message>
adding final results expression analysis
</commit_message>
<xml_diff>
--- a/real_data/3_differential_expression_analysis/summary/summary_results.xlsx
+++ b/real_data/3_differential_expression_analysis/summary/summary_results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniele/Desktop/differential_expression_analysis/summary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniele/Documents/BIMIB/LACE-UTILITIES/real_data/3_differential_expression_analysis/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E320C1E-6AA5-6946-8B43-DEEB81FEDFFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AAB896B-11FD-DD4F-90B5-EFFBB3202A08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="1020" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="355">
   <si>
     <t>ensembl_gene_id</t>
   </si>
@@ -1078,6 +1078,15 @@
   </si>
   <si>
     <t>pvalues_fdr</t>
+  </si>
+  <si>
+    <t>ENSG00000212296</t>
+  </si>
+  <si>
+    <t>SNORD72</t>
+  </si>
+  <si>
+    <t>snoRNA</t>
   </si>
 </sst>
 </file>
@@ -1971,7 +1980,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="4">
-        <v>5.1047187002619104E-3</v>
+        <v>3.14273722313044E-3</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
@@ -1985,7 +1994,7 @@
         <v>5</v>
       </c>
       <c r="E4" s="4">
-        <v>0.10660302099989399</v>
+        <v>0.117134290697176</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
@@ -1999,217 +2008,217 @@
         <v>5</v>
       </c>
       <c r="E5" s="4">
-        <v>0.10660302099989399</v>
+        <v>0.117134290697176</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="4">
-        <v>0.14721684249702</v>
+        <v>0.14762696251559901</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="4">
-        <v>0.14721684249702</v>
+        <v>0.14762696251559901</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>72</v>
+        <v>13</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="4">
-        <v>0.14721684249702</v>
+        <v>0.14762696251559901</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>116</v>
+        <v>7</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="4">
-        <v>0.14721684249702</v>
+        <v>0.14762696251559901</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>118</v>
+        <v>42</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="4">
-        <v>0.14721684249702</v>
+        <v>0.14762696251559901</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="4">
-        <v>0.14721684249702</v>
+        <v>0.14762696251559901</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>79</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="4">
-        <v>0.164545853115207</v>
+        <v>0.14762696251559901</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>114</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E13" s="4">
-        <v>0.164545853115207</v>
+        <v>0.14762696251559901</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="4">
-        <v>0.164545853115207</v>
+        <v>0.14762696251559901</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>46</v>
+        <v>118</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E15" s="4">
-        <v>0.164545853115207</v>
+        <v>0.14762696251559901</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E16" s="4">
-        <v>0.166227080634439</v>
+        <v>0.14762696251559901</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>119</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="4">
-        <v>0.166227080634439</v>
+        <v>0.14762696251559901</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>67</v>
+        <v>352</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>68</v>
+        <v>353</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>5</v>
+        <v>354</v>
       </c>
       <c r="E18" s="4">
-        <v>0.17886138958134001</v>
+        <v>0.14762696251559901</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>121</v>
+        <v>45</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>122</v>
+        <v>46</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="4">
-        <v>0.17886138958134001</v>
+        <v>0.154836522959376</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>18</v>
+        <v>121</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>19</v>
+        <v>122</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E20" s="4">
-        <v>0.19299376825483799</v>
+        <v>0.16298343008038799</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
@@ -2223,25 +2232,36 @@
         <v>5</v>
       </c>
       <c r="E21" s="4">
-        <v>0.19299376825483799</v>
+        <v>0.170564291484817</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0.17377492484991899</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="4">
-        <v>0.19299376825483799</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.18531549060969599</v>
+      </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D24" s="3"/>

</xml_diff>